<commit_message>
IPS 337-Carga VMP parte 1
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/IndicadoresPlanoTrabalho.xlsx
+++ b/Gestão do Projeto/Indicadores/IndicadoresPlanoTrabalho.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B374CB22-C4FC-7747-A759-A075370F6113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AF7469-6D60-074F-B67A-DBF3092783BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="760" windowWidth="26840" windowHeight="15940" xr2:uid="{BBEB64F3-A0FD-8443-B46C-44F3CC52CE04}"/>
+    <workbookView xWindow="2400" yWindow="1100" windowWidth="26840" windowHeight="15940" xr2:uid="{BBEB64F3-A0FD-8443-B46C-44F3CC52CE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Indicadores de resultado do projeto</t>
   </si>
@@ -50,9 +54,6 @@
     <t>Metas</t>
   </si>
   <si>
-    <t>meses</t>
-  </si>
-  <si>
     <t xml:space="preserve">% de terminologias e domínios locais do bloco imunização e mapeamentos (mapas de conceitos) para as terminologias do IPS carregados no serviço de terminologia   </t>
   </si>
   <si>
@@ -75,6 +76,15 @@
   </si>
   <si>
     <t xml:space="preserve">% do Guia de Implementação do Brasil IPS especificado e aderente aos padrões HL7 FHIR IG IPS </t>
+  </si>
+  <si>
+    <t>Situação Abril 2023</t>
+  </si>
+  <si>
+    <t>meses (junho 23)</t>
+  </si>
+  <si>
+    <t>meses (dez23)</t>
   </si>
 </sst>
 </file>
@@ -128,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,8 +157,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -181,19 +203,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -292,92 +301,140 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -394,6 +451,46 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tarefas"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="U2">
+            <v>0.82954545454545459</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Março-23"/>
+      <sheetName val="Abril-23"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="T2">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C209F-BEDB-6A41-9AE1-7109A510D013}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:E13"/>
+    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,223 +801,239 @@
     <col min="2" max="2" width="36.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="32" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="1"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6">
         <v>6</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="27">
         <v>12</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="15"/>
+        <v>13</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>6</v>
       </c>
       <c r="D5" s="9">
         <v>50</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="28">
         <v>100</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="33">
+        <f>'[2]Abril-23'!$T$2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="9">
         <v>50</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="28">
         <v>100</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="9">
         <v>50</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="28">
         <v>100</v>
       </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="34">
+        <f>[1]Tarefas!$U$2</f>
+        <v>0.82954545454545459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="9">
         <v>50</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="28">
         <v>100</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="9">
         <v>40</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="28">
         <v>100</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="11">
+        <v>20</v>
+      </c>
+      <c r="E10" s="29">
+        <v>100</v>
+      </c>
+      <c r="F10" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
         <v>6</v>
       </c>
-      <c r="D10" s="13">
-        <v>20</v>
-      </c>
-      <c r="E10" s="13">
-        <v>100</v>
-      </c>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>6</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="13">
+      <c r="B12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="11">
         <v>0</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="29">
         <v>1</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Indicadores e Atas atualizadas
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/IndicadoresPlanoTrabalho.xlsx
+++ b/Gestão do Projeto/Indicadores/IndicadoresPlanoTrabalho.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61480B36-F1FB-C942-9E4B-A466E34477EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDE5CB2-54A6-424F-AD4F-C170D465193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="1280" windowWidth="26840" windowHeight="15940" xr2:uid="{BBEB64F3-A0FD-8443-B46C-44F3CC52CE04}"/>
+    <workbookView xWindow="2300" yWindow="2140" windowWidth="26840" windowHeight="15940" xr2:uid="{BBEB64F3-A0FD-8443-B46C-44F3CC52CE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,121 +170,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -303,150 +193,69 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C209F-BEDB-6A41-9AE1-7109A510D013}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,218 +625,218 @@
     <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="29" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="29"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="14">
         <v>6</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="14">
         <v>12</v>
       </c>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="29"/>
-    </row>
-    <row r="5" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="4">
         <v>50</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="4">
         <v>100</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="3">
         <f>'[1]Abril-23'!$T$2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A6" s="20">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="4">
         <v>50</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="4">
         <v>100</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="2">
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="4">
         <v>50</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="4">
         <v>100</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="2">
         <f>[2]Tarefas!$U$2</f>
         <v>0.82954545454545459</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    <row r="8" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="4">
         <v>50</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="4">
         <v>100</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="5">
         <v>0.46899999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="6">
         <v>4</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="4">
         <v>40</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="4">
         <v>100</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34">
+      <c r="A10" s="10">
         <v>5</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="9">
         <v>20</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="9">
         <v>100</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="7">
         <v>0.46</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="28"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32">
+      <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="9">
         <v>0</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="9">
         <v>2</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="28"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="5"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>